<commit_message>
Corrected definitions, TODO: new argument `calculate_score_change_with_break_in_series` in JAF_output
</commit_message>
<xml_diff>
--- a/JAF_indicators__definitions.xlsx
+++ b/JAF_indicators__definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/JAF2R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="11_8EB80073D8E76818760C99562770445F322C70A0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{110EBEEC-0237-45E7-857F-33364781497A}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="11_8EB80073D8E76818760C99562770445F322C70A0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{491490BB-75BF-4589-B1E9-1636ABB3AB2F}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7662,7 +7662,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="jaf" displayName="jaf" ref="A2:J648" totalsRowShown="0">
-  <autoFilter ref="A2:J648" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A2:J648" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="JAF_KEY"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -8078,7 +8084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -8138,7 +8144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -8198,7 +8204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -8258,7 +8264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -8318,7 +8324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -8378,7 +8384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -8438,7 +8444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -8498,7 +8504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -8558,7 +8564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -8618,7 +8624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -8678,7 +8684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -8738,7 +8744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -8798,7 +8804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -8858,7 +8864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -8918,7 +8924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -8978,7 +8984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -9038,7 +9044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -9098,7 +9104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -9158,7 +9164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -9218,7 +9224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -9278,7 +9284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -9338,7 +9344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -9398,7 +9404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -9458,7 +9464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -9518,7 +9524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -9578,7 +9584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -9638,7 +9644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -9698,7 +9704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -9758,7 +9764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>141</v>
       </c>
@@ -9818,7 +9824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -9878,7 +9884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -9938,7 +9944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -9998,7 +10004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -10058,7 +10064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -10118,7 +10124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -10178,7 +10184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -10238,7 +10244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>173</v>
       </c>
@@ -10298,7 +10304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>177</v>
       </c>
@@ -10358,7 +10364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -10418,7 +10424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>185</v>
       </c>
@@ -10478,7 +10484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>189</v>
       </c>
@@ -10538,7 +10544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>193</v>
       </c>
@@ -10598,7 +10604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>197</v>
       </c>
@@ -10658,7 +10664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>201</v>
       </c>
@@ -10718,7 +10724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>205</v>
       </c>
@@ -10778,7 +10784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -10838,7 +10844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>213</v>
       </c>
@@ -10898,7 +10904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>217</v>
       </c>
@@ -10958,7 +10964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -11018,7 +11024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -11078,7 +11084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -11138,7 +11144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>232</v>
       </c>
@@ -11198,7 +11204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>236</v>
       </c>
@@ -11258,7 +11264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -11318,7 +11324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>245</v>
       </c>
@@ -11378,7 +11384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -11438,7 +11444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>251</v>
       </c>
@@ -11498,7 +11504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>254</v>
       </c>
@@ -11558,7 +11564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>257</v>
       </c>
@@ -11618,7 +11624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>260</v>
       </c>
@@ -11678,7 +11684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>263</v>
       </c>
@@ -11738,7 +11744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>266</v>
       </c>
@@ -11798,7 +11804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>269</v>
       </c>
@@ -11858,7 +11864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>272</v>
       </c>
@@ -11918,7 +11924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>275</v>
       </c>
@@ -11978,7 +11984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>278</v>
       </c>
@@ -12038,7 +12044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>281</v>
       </c>
@@ -12098,7 +12104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>284</v>
       </c>
@@ -12158,7 +12164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -12218,7 +12224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>290</v>
       </c>
@@ -12278,7 +12284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>293</v>
       </c>
@@ -12338,7 +12344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>296</v>
       </c>
@@ -12398,7 +12404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>299</v>
       </c>
@@ -12458,7 +12464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>303</v>
       </c>
@@ -12518,7 +12524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>307</v>
       </c>
@@ -12578,7 +12584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>311</v>
       </c>
@@ -12638,7 +12644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>315</v>
       </c>
@@ -12698,7 +12704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>319</v>
       </c>
@@ -12758,7 +12764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>323</v>
       </c>
@@ -12818,7 +12824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>326</v>
       </c>
@@ -12878,7 +12884,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>329</v>
       </c>
@@ -12938,7 +12944,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>333</v>
       </c>
@@ -12998,7 +13004,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>337</v>
       </c>
@@ -13058,7 +13064,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>340</v>
       </c>
@@ -13118,7 +13124,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>344</v>
       </c>
@@ -13178,7 +13184,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>348</v>
       </c>
@@ -13238,7 +13244,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>351</v>
       </c>
@@ -13298,7 +13304,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>354</v>
       </c>
@@ -13358,7 +13364,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>359</v>
       </c>
@@ -13418,7 +13424,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>362</v>
       </c>
@@ -13478,7 +13484,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>365</v>
       </c>
@@ -13538,7 +13544,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>368</v>
       </c>
@@ -13598,7 +13604,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>371</v>
       </c>
@@ -13658,7 +13664,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>375</v>
       </c>
@@ -13718,7 +13724,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>378</v>
       </c>
@@ -13778,7 +13784,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>381</v>
       </c>
@@ -13838,7 +13844,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>385</v>
       </c>
@@ -13898,7 +13904,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>389</v>
       </c>
@@ -13958,7 +13964,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>393</v>
       </c>
@@ -14018,7 +14024,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>397</v>
       </c>
@@ -14078,7 +14084,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>401</v>
       </c>
@@ -14138,7 +14144,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>405</v>
       </c>
@@ -14198,7 +14204,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>409</v>
       </c>
@@ -14258,7 +14264,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>413</v>
       </c>
@@ -14318,7 +14324,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>417</v>
       </c>
@@ -14378,7 +14384,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>421</v>
       </c>
@@ -14438,7 +14444,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>425</v>
       </c>
@@ -14498,7 +14504,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>429</v>
       </c>
@@ -14558,7 +14564,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>432</v>
       </c>
@@ -14618,7 +14624,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>435</v>
       </c>
@@ -14678,7 +14684,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>438</v>
       </c>
@@ -14738,7 +14744,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>441</v>
       </c>
@@ -14798,7 +14804,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>444</v>
       </c>
@@ -14858,7 +14864,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>447</v>
       </c>
@@ -14918,7 +14924,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>450</v>
       </c>
@@ -14978,7 +14984,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>453</v>
       </c>
@@ -15038,7 +15044,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>457</v>
       </c>
@@ -15098,7 +15104,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>460</v>
       </c>
@@ -15158,7 +15164,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>463</v>
       </c>
@@ -15218,7 +15224,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>466</v>
       </c>
@@ -15278,7 +15284,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>467</v>
       </c>
@@ -15338,7 +15344,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>469</v>
       </c>
@@ -15398,7 +15404,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>473</v>
       </c>
@@ -15458,7 +15464,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>477</v>
       </c>
@@ -15518,7 +15524,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>481</v>
       </c>
@@ -15578,7 +15584,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>482</v>
       </c>
@@ -15638,7 +15644,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>487</v>
       </c>
@@ -15698,7 +15704,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>490</v>
       </c>
@@ -15758,7 +15764,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>493</v>
       </c>
@@ -15818,7 +15824,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>496</v>
       </c>
@@ -15878,7 +15884,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>500</v>
       </c>
@@ -15938,7 +15944,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>504</v>
       </c>
@@ -15998,7 +16004,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>508</v>
       </c>
@@ -16058,7 +16064,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>513</v>
       </c>
@@ -16118,7 +16124,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>517</v>
       </c>
@@ -16178,7 +16184,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>520</v>
       </c>
@@ -16238,7 +16244,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>524</v>
       </c>
@@ -16298,7 +16304,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>527</v>
       </c>
@@ -16358,7 +16364,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>531</v>
       </c>
@@ -16418,7 +16424,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>534</v>
       </c>
@@ -16478,7 +16484,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>537</v>
       </c>
@@ -16538,7 +16544,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>541</v>
       </c>
@@ -16598,7 +16604,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>545</v>
       </c>
@@ -16658,7 +16664,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>549</v>
       </c>
@@ -16718,7 +16724,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>553</v>
       </c>
@@ -16778,7 +16784,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>557</v>
       </c>
@@ -16838,7 +16844,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>561</v>
       </c>
@@ -16898,7 +16904,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>562</v>
       </c>
@@ -16958,7 +16964,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>566</v>
       </c>
@@ -17018,7 +17024,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>567</v>
       </c>
@@ -17078,7 +17084,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>570</v>
       </c>
@@ -17138,7 +17144,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>573</v>
       </c>
@@ -17198,7 +17204,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>576</v>
       </c>
@@ -17258,7 +17264,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>580</v>
       </c>
@@ -17318,7 +17324,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>584</v>
       </c>
@@ -17378,7 +17384,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>588</v>
       </c>
@@ -17438,7 +17444,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>591</v>
       </c>
@@ -17498,7 +17504,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>595</v>
       </c>
@@ -17558,7 +17564,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>598</v>
       </c>
@@ -17618,7 +17624,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>601</v>
       </c>
@@ -17678,7 +17684,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>604</v>
       </c>
@@ -17738,7 +17744,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>606</v>
       </c>
@@ -17798,7 +17804,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>610</v>
       </c>
@@ -17858,7 +17864,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>614</v>
       </c>
@@ -17918,7 +17924,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>618</v>
       </c>
@@ -17978,7 +17984,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>622</v>
       </c>
@@ -18038,7 +18044,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>626</v>
       </c>
@@ -18098,7 +18104,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>630</v>
       </c>
@@ -18158,7 +18164,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>634</v>
       </c>
@@ -18218,7 +18224,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>638</v>
       </c>
@@ -18278,7 +18284,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>642</v>
       </c>
@@ -18338,7 +18344,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>646</v>
       </c>
@@ -18398,7 +18404,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>650</v>
       </c>
@@ -18458,7 +18464,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>653</v>
       </c>
@@ -18518,7 +18524,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>656</v>
       </c>
@@ -18578,7 +18584,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>659</v>
       </c>
@@ -18638,7 +18644,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>662</v>
       </c>
@@ -18698,7 +18704,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>665</v>
       </c>
@@ -18758,7 +18764,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>668</v>
       </c>
@@ -18818,7 +18824,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>672</v>
       </c>
@@ -18878,7 +18884,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>676</v>
       </c>
@@ -18938,7 +18944,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>680</v>
       </c>
@@ -18998,7 +19004,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>684</v>
       </c>
@@ -19058,7 +19064,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>688</v>
       </c>
@@ -19118,7 +19124,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>692</v>
       </c>
@@ -19178,7 +19184,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>697</v>
       </c>
@@ -19238,7 +19244,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>702</v>
       </c>
@@ -19298,7 +19304,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>706</v>
       </c>
@@ -19358,7 +19364,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>710</v>
       </c>
@@ -19418,7 +19424,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>714</v>
       </c>
@@ -19478,7 +19484,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>718</v>
       </c>
@@ -19538,7 +19544,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>721</v>
       </c>
@@ -19598,7 +19604,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>725</v>
       </c>
@@ -19658,7 +19664,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>729</v>
       </c>
@@ -19718,7 +19724,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>733</v>
       </c>
@@ -19778,7 +19784,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>737</v>
       </c>
@@ -19838,7 +19844,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>741</v>
       </c>
@@ -19898,7 +19904,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>745</v>
       </c>
@@ -19958,7 +19964,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>751</v>
       </c>
@@ -20018,7 +20024,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>757</v>
       </c>
@@ -20078,7 +20084,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>760</v>
       </c>
@@ -20138,7 +20144,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>764</v>
       </c>
@@ -20198,7 +20204,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>768</v>
       </c>
@@ -20258,7 +20264,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>771</v>
       </c>
@@ -20318,7 +20324,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>775</v>
       </c>
@@ -20378,7 +20384,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>779</v>
       </c>
@@ -20438,7 +20444,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>783</v>
       </c>
@@ -20498,7 +20504,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>787</v>
       </c>
@@ -20558,7 +20564,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>791</v>
       </c>
@@ -20618,7 +20624,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>795</v>
       </c>
@@ -20678,7 +20684,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>798</v>
       </c>
@@ -20738,7 +20744,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>802</v>
       </c>
@@ -20798,7 +20804,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>805</v>
       </c>
@@ -20858,7 +20864,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>808</v>
       </c>
@@ -20918,7 +20924,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>811</v>
       </c>
@@ -20978,7 +20984,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>815</v>
       </c>
@@ -21038,7 +21044,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>818</v>
       </c>
@@ -21098,7 +21104,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>822</v>
       </c>
@@ -21158,7 +21164,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>826</v>
       </c>
@@ -21218,7 +21224,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>827</v>
       </c>
@@ -21278,7 +21284,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>829</v>
       </c>
@@ -21338,7 +21344,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>833</v>
       </c>
@@ -21398,7 +21404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>835</v>
       </c>
@@ -21458,7 +21464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>839</v>
       </c>
@@ -21578,7 +21584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>848</v>
       </c>
@@ -21638,7 +21644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>852</v>
       </c>
@@ -21698,7 +21704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>856</v>
       </c>
@@ -21758,7 +21764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>861</v>
       </c>
@@ -21818,7 +21824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>864</v>
       </c>
@@ -21878,7 +21884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>867</v>
       </c>
@@ -21938,7 +21944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>870</v>
       </c>
@@ -21998,7 +22004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>873</v>
       </c>
@@ -22058,7 +22064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>876</v>
       </c>
@@ -22118,7 +22124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>879</v>
       </c>
@@ -22238,7 +22244,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>886</v>
       </c>
@@ -22298,7 +22304,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>889</v>
       </c>
@@ -22358,7 +22364,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>894</v>
       </c>
@@ -22418,7 +22424,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>897</v>
       </c>
@@ -22478,7 +22484,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>900</v>
       </c>
@@ -22538,7 +22544,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>903</v>
       </c>
@@ -22598,7 +22604,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>906</v>
       </c>
@@ -22658,7 +22664,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>909</v>
       </c>
@@ -22718,7 +22724,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>912</v>
       </c>
@@ -22778,7 +22784,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>915</v>
       </c>
@@ -22838,7 +22844,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>919</v>
       </c>
@@ -22898,7 +22904,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>922</v>
       </c>
@@ -22958,7 +22964,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>925</v>
       </c>
@@ -23078,7 +23084,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>934</v>
       </c>
@@ -23138,7 +23144,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>939</v>
       </c>
@@ -23198,7 +23204,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>943</v>
       </c>
@@ -23258,7 +23264,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>946</v>
       </c>
@@ -23318,7 +23324,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>949</v>
       </c>
@@ -23378,7 +23384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>953</v>
       </c>
@@ -23438,7 +23444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>957</v>
       </c>
@@ -23498,7 +23504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>960</v>
       </c>
@@ -23558,7 +23564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>963</v>
       </c>
@@ -23618,7 +23624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>966</v>
       </c>
@@ -23678,7 +23684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>970</v>
       </c>
@@ -23738,7 +23744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>975</v>
       </c>
@@ -23798,7 +23804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>978</v>
       </c>
@@ -23858,7 +23864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>981</v>
       </c>
@@ -23918,7 +23924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>984</v>
       </c>
@@ -23978,7 +23984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>987</v>
       </c>
@@ -24038,7 +24044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>990</v>
       </c>
@@ -24098,7 +24104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>993</v>
       </c>
@@ -24158,7 +24164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>997</v>
       </c>
@@ -24218,7 +24224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>1001</v>
       </c>
@@ -24278,7 +24284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>1004</v>
       </c>
@@ -24338,7 +24344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>1007</v>
       </c>
@@ -24398,7 +24404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>1010</v>
       </c>
@@ -24458,7 +24464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>1014</v>
       </c>
@@ -25058,7 +25064,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>1048</v>
       </c>
@@ -25118,7 +25124,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>1052</v>
       </c>
@@ -25178,7 +25184,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>1057</v>
       </c>
@@ -25238,7 +25244,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>1060</v>
       </c>
@@ -25298,7 +25304,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>1063</v>
       </c>
@@ -25358,7 +25364,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>1066</v>
       </c>
@@ -25418,7 +25424,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>1069</v>
       </c>
@@ -25478,7 +25484,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>1072</v>
       </c>
@@ -25538,7 +25544,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>1075</v>
       </c>
@@ -25598,7 +25604,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>1078</v>
       </c>
@@ -25658,7 +25664,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>1082</v>
       </c>
@@ -25718,7 +25724,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>1086</v>
       </c>
@@ -25778,7 +25784,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>1090</v>
       </c>
@@ -25838,7 +25844,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>1094</v>
       </c>
@@ -25898,7 +25904,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>1097</v>
       </c>
@@ -25958,7 +25964,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>1102</v>
       </c>
@@ -26018,7 +26024,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>1107</v>
       </c>
@@ -26078,7 +26084,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>1111</v>
       </c>
@@ -26198,7 +26204,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>1116</v>
       </c>
@@ -26258,7 +26264,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>1120</v>
       </c>
@@ -26318,7 +26324,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>1125</v>
       </c>
@@ -26378,7 +26384,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>1130</v>
       </c>
@@ -26438,7 +26444,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>1134</v>
       </c>
@@ -26498,7 +26504,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
         <v>1138</v>
       </c>
@@ -26558,7 +26564,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>1142</v>
       </c>
@@ -26618,7 +26624,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>1146</v>
       </c>
@@ -26678,7 +26684,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>1150</v>
       </c>
@@ -26738,7 +26744,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>1152</v>
       </c>
@@ -26798,7 +26804,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>1154</v>
       </c>
@@ -26858,7 +26864,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>1158</v>
       </c>
@@ -26918,7 +26924,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>1163</v>
       </c>
@@ -26978,7 +26984,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>1165</v>
       </c>
@@ -27038,7 +27044,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>1169</v>
       </c>
@@ -27098,7 +27104,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>1172</v>
       </c>
@@ -27158,7 +27164,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>1175</v>
       </c>
@@ -27218,7 +27224,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A322" t="s">
         <v>1180</v>
       </c>
@@ -27278,7 +27284,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>1181</v>
       </c>
@@ -27338,7 +27344,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A324" t="s">
         <v>1184</v>
       </c>
@@ -27398,7 +27404,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>1187</v>
       </c>
@@ -27458,7 +27464,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A326" t="s">
         <v>1190</v>
       </c>
@@ -27518,7 +27524,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>1193</v>
       </c>
@@ -27578,7 +27584,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A328" t="s">
         <v>1194</v>
       </c>
@@ -27638,7 +27644,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>1195</v>
       </c>
@@ -27698,7 +27704,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A330" t="s">
         <v>1196</v>
       </c>
@@ -27758,7 +27764,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>1197</v>
       </c>
@@ -27818,7 +27824,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>1202</v>
       </c>
@@ -27878,7 +27884,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>1206</v>
       </c>
@@ -27938,7 +27944,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A334" t="s">
         <v>1209</v>
       </c>
@@ -27998,7 +28004,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>1213</v>
       </c>
@@ -28118,7 +28124,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>1223</v>
       </c>
@@ -28178,7 +28184,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A338" t="s">
         <v>1228</v>
       </c>
@@ -28238,7 +28244,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>1231</v>
       </c>
@@ -28298,7 +28304,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
         <v>1236</v>
       </c>
@@ -28358,7 +28364,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>1239</v>
       </c>
@@ -28418,7 +28424,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>1243</v>
       </c>
@@ -28478,7 +28484,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>1247</v>
       </c>
@@ -28538,7 +28544,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>1251</v>
       </c>
@@ -28598,7 +28604,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>1256</v>
       </c>
@@ -28658,7 +28664,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>1260</v>
       </c>
@@ -28718,7 +28724,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>1264</v>
       </c>
@@ -28778,7 +28784,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>1268</v>
       </c>
@@ -28838,7 +28844,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>1272</v>
       </c>
@@ -28898,7 +28904,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>1276</v>
       </c>
@@ -28958,7 +28964,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>1280</v>
       </c>
@@ -29018,7 +29024,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>1285</v>
       </c>
@@ -29078,7 +29084,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>1289</v>
       </c>
@@ -29138,7 +29144,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A354" t="s">
         <v>1293</v>
       </c>
@@ -29198,7 +29204,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>1297</v>
       </c>
@@ -29258,7 +29264,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
         <v>1300</v>
       </c>
@@ -29318,7 +29324,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>1304</v>
       </c>
@@ -29378,7 +29384,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>1308</v>
       </c>
@@ -29438,7 +29444,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>1312</v>
       </c>
@@ -29498,7 +29504,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A360" t="s">
         <v>1316</v>
       </c>
@@ -29558,7 +29564,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>1320</v>
       </c>
@@ -29618,7 +29624,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>1324</v>
       </c>
@@ -29678,7 +29684,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>1327</v>
       </c>
@@ -29738,7 +29744,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
         <v>1330</v>
       </c>
@@ -29798,7 +29804,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A365" t="s">
         <v>1332</v>
       </c>
@@ -29858,7 +29864,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A366" t="s">
         <v>1337</v>
       </c>
@@ -29918,7 +29924,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
         <v>1341</v>
       </c>
@@ -29978,7 +29984,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A368" t="s">
         <v>1343</v>
       </c>
@@ -30038,7 +30044,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A369" t="s">
         <v>1345</v>
       </c>
@@ -30098,7 +30104,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A370" t="s">
         <v>1348</v>
       </c>
@@ -30158,7 +30164,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A371" t="s">
         <v>1351</v>
       </c>
@@ -30218,7 +30224,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A372" t="s">
         <v>1355</v>
       </c>
@@ -30278,7 +30284,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A373" t="s">
         <v>1359</v>
       </c>
@@ -30338,7 +30344,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A374" t="s">
         <v>1363</v>
       </c>
@@ -30398,7 +30404,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A375" t="s">
         <v>1367</v>
       </c>
@@ -30458,7 +30464,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A376" t="s">
         <v>1370</v>
       </c>
@@ -30518,7 +30524,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A377" t="s">
         <v>1374</v>
       </c>
@@ -30578,7 +30584,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A378" t="s">
         <v>1378</v>
       </c>
@@ -30638,7 +30644,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A379" t="s">
         <v>1382</v>
       </c>
@@ -30698,7 +30704,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A380" t="s">
         <v>1386</v>
       </c>
@@ -30758,7 +30764,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A381" t="s">
         <v>1388</v>
       </c>
@@ -30818,7 +30824,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A382" t="s">
         <v>1390</v>
       </c>
@@ -30878,7 +30884,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
         <v>1392</v>
       </c>
@@ -30938,7 +30944,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A384" t="s">
         <v>1394</v>
       </c>
@@ -30998,7 +31004,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>1397</v>
       </c>
@@ -31058,7 +31064,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A386" t="s">
         <v>1400</v>
       </c>
@@ -31118,7 +31124,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A387" t="s">
         <v>1403</v>
       </c>
@@ -31178,7 +31184,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A388" t="s">
         <v>1406</v>
       </c>
@@ -31238,7 +31244,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A389" t="s">
         <v>1411</v>
       </c>
@@ -31298,7 +31304,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A390" t="s">
         <v>1416</v>
       </c>
@@ -31358,7 +31364,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A391" t="s">
         <v>1419</v>
       </c>
@@ -31418,7 +31424,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A392" t="s">
         <v>1422</v>
       </c>
@@ -31478,7 +31484,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A393" t="s">
         <v>1425</v>
       </c>
@@ -31538,7 +31544,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A394" t="s">
         <v>1428</v>
       </c>
@@ -31598,7 +31604,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>1431</v>
       </c>
@@ -31658,7 +31664,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A396" t="s">
         <v>1435</v>
       </c>
@@ -31718,7 +31724,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A397" t="s">
         <v>1439</v>
       </c>
@@ -31778,7 +31784,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A398" t="s">
         <v>1443</v>
       </c>
@@ -31838,7 +31844,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
         <v>1447</v>
       </c>
@@ -31898,7 +31904,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A400" t="s">
         <v>1450</v>
       </c>
@@ -31958,7 +31964,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A401" t="s">
         <v>1453</v>
       </c>
@@ -32018,7 +32024,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A402" t="s">
         <v>1456</v>
       </c>
@@ -32078,7 +32084,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A403" t="s">
         <v>1459</v>
       </c>
@@ -32138,7 +32144,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A404" t="s">
         <v>1462</v>
       </c>
@@ -32198,7 +32204,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A405" t="s">
         <v>1465</v>
       </c>
@@ -32258,7 +32264,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A406" t="s">
         <v>1468</v>
       </c>
@@ -32318,7 +32324,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A407" t="s">
         <v>1472</v>
       </c>
@@ -32378,7 +32384,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A408" t="s">
         <v>1475</v>
       </c>
@@ -32618,7 +32624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A412" t="s">
         <v>1485</v>
       </c>
@@ -32678,7 +32684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A413" t="s">
         <v>1488</v>
       </c>
@@ -33218,7 +33224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A422" t="s">
         <v>1514</v>
       </c>
@@ -33278,7 +33284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A423" t="s">
         <v>1517</v>
       </c>
@@ -33338,7 +33344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A424" t="s">
         <v>1519</v>
       </c>
@@ -33398,7 +33404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A425" t="s">
         <v>1522</v>
       </c>
@@ -33458,7 +33464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="426" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A426" t="s">
         <v>1525</v>
       </c>
@@ -33518,7 +33524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="427" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A427" t="s">
         <v>1530</v>
       </c>
@@ -33578,7 +33584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="428" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A428" t="s">
         <v>1532</v>
       </c>
@@ -33638,7 +33644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="429" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A429" t="s">
         <v>1536</v>
       </c>
@@ -33698,7 +33704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="430" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A430" t="s">
         <v>1537</v>
       </c>
@@ -33758,7 +33764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="431" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A431" t="s">
         <v>1540</v>
       </c>
@@ -34778,7 +34784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="448" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A448" t="s">
         <v>1587</v>
       </c>
@@ -34838,7 +34844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="449" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A449" t="s">
         <v>1590</v>
       </c>
@@ -34958,7 +34964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="451" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A451" t="s">
         <v>1594</v>
       </c>
@@ -35018,7 +35024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="452" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A452" t="s">
         <v>1597</v>
       </c>
@@ -35078,7 +35084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="453" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A453" t="s">
         <v>1598</v>
       </c>
@@ -35198,7 +35204,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="455" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A455" t="s">
         <v>1605</v>
       </c>
@@ -35258,7 +35264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="456" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A456" t="s">
         <v>1610</v>
       </c>
@@ -35318,7 +35324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="457" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A457" t="s">
         <v>1614</v>
       </c>
@@ -35378,7 +35384,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="458" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A458" t="s">
         <v>1618</v>
       </c>
@@ -35438,7 +35444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="459" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A459" t="s">
         <v>1623</v>
       </c>
@@ -35498,7 +35504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="460" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A460" t="s">
         <v>1626</v>
       </c>
@@ -35558,7 +35564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="461" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A461" t="s">
         <v>1629</v>
       </c>
@@ -35618,7 +35624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="462" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A462" t="s">
         <v>1632</v>
       </c>
@@ -35678,7 +35684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="463" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A463" t="s">
         <v>1635</v>
       </c>
@@ -35738,7 +35744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="464" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A464" t="s">
         <v>1638</v>
       </c>
@@ -35798,7 +35804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="465" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A465" t="s">
         <v>1641</v>
       </c>
@@ -35858,7 +35864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="466" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A466" t="s">
         <v>1644</v>
       </c>
@@ -35918,7 +35924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="467" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A467" t="s">
         <v>1647</v>
       </c>
@@ -35978,7 +35984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="468" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A468" t="s">
         <v>1650</v>
       </c>
@@ -36038,7 +36044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="469" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A469" t="s">
         <v>1653</v>
       </c>
@@ -36098,7 +36104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="470" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A470" t="s">
         <v>1656</v>
       </c>
@@ -36158,7 +36164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="471" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A471" t="s">
         <v>1659</v>
       </c>
@@ -36218,7 +36224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="472" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="472" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A472" t="s">
         <v>1662</v>
       </c>
@@ -36278,7 +36284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="473" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A473" t="s">
         <v>1665</v>
       </c>
@@ -36338,7 +36344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="474" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="474" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A474" t="s">
         <v>1668</v>
       </c>
@@ -36398,7 +36404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="475" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="475" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A475" t="s">
         <v>1672</v>
       </c>
@@ -36458,7 +36464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="476" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="476" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A476" t="s">
         <v>1675</v>
       </c>
@@ -36518,7 +36524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="477" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="477" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A477" t="s">
         <v>1678</v>
       </c>
@@ -36578,7 +36584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="478" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="478" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A478" t="s">
         <v>1681</v>
       </c>
@@ -36638,7 +36644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="479" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A479" t="s">
         <v>1685</v>
       </c>
@@ -36698,7 +36704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="480" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="480" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A480" t="s">
         <v>1688</v>
       </c>
@@ -36998,7 +37004,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="485" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="485" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A485" t="s">
         <v>1702</v>
       </c>
@@ -37058,7 +37064,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="486" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="486" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A486" t="s">
         <v>1705</v>
       </c>
@@ -37118,7 +37124,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="487" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="487" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A487" t="s">
         <v>1708</v>
       </c>
@@ -37178,7 +37184,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="488" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="488" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A488" t="s">
         <v>1711</v>
       </c>
@@ -37718,7 +37724,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="497" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="497" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A497" t="s">
         <v>1732</v>
       </c>
@@ -37778,7 +37784,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="498" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="498" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A498" t="s">
         <v>1735</v>
       </c>
@@ -37958,7 +37964,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="501" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="501" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A501" t="s">
         <v>1742</v>
       </c>
@@ -38138,7 +38144,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="504" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="504" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A504" t="s">
         <v>1751</v>
       </c>
@@ -38198,7 +38204,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="505" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="505" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A505" t="s">
         <v>1754</v>
       </c>
@@ -38258,7 +38264,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="506" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="506" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A506" t="s">
         <v>1756</v>
       </c>
@@ -38318,7 +38324,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="507" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="507" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A507" t="s">
         <v>1759</v>
       </c>
@@ -38378,7 +38384,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="508" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="508" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A508" t="s">
         <v>1761</v>
       </c>
@@ -38438,7 +38444,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="509" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="509" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A509" t="s">
         <v>1765</v>
       </c>
@@ -38498,7 +38504,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="510" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="510" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A510" t="s">
         <v>1768</v>
       </c>
@@ -38798,7 +38804,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="515" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="515" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A515" t="s">
         <v>1781</v>
       </c>
@@ -38858,7 +38864,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="516" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="516" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A516" t="s">
         <v>1784</v>
       </c>
@@ -38918,7 +38924,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="517" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="517" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A517" t="s">
         <v>1787</v>
       </c>
@@ -38978,7 +38984,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="518" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="518" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A518" t="s">
         <v>1790</v>
       </c>
@@ -39038,7 +39044,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="519" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="519" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A519" t="s">
         <v>1794</v>
       </c>
@@ -39098,7 +39104,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="520" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="520" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A520" t="s">
         <v>1795</v>
       </c>
@@ -39998,7 +40004,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="535" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="535" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A535" t="s">
         <v>1829</v>
       </c>
@@ -40058,7 +40064,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="536" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="536" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A536" t="s">
         <v>1832</v>
       </c>
@@ -40118,7 +40124,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="537" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="537" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A537" t="s">
         <v>1833</v>
       </c>
@@ -40178,7 +40184,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="538" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="538" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A538" t="s">
         <v>1836</v>
       </c>
@@ -40238,7 +40244,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="539" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="539" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A539" t="s">
         <v>1839</v>
       </c>
@@ -40298,7 +40304,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="540" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="540" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A540" t="s">
         <v>1840</v>
       </c>
@@ -40358,7 +40364,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="541" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="541" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A541" t="s">
         <v>1842</v>
       </c>
@@ -40418,7 +40424,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="542" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="542" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A542" t="s">
         <v>1845</v>
       </c>
@@ -40478,7 +40484,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="543" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="543" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A543" t="s">
         <v>1848</v>
       </c>
@@ -40538,7 +40544,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="544" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="544" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A544" t="s">
         <v>1851</v>
       </c>
@@ -41198,7 +41204,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="555" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="555" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A555" t="s">
         <v>1879</v>
       </c>
@@ -41258,7 +41264,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="556" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="556" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A556" t="s">
         <v>1882</v>
       </c>
@@ -41318,7 +41324,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="557" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="557" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A557" t="s">
         <v>1885</v>
       </c>
@@ -41378,7 +41384,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="558" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="558" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A558" t="s">
         <v>1888</v>
       </c>
@@ -41438,7 +41444,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="559" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="559" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A559" t="s">
         <v>1891</v>
       </c>
@@ -41498,7 +41504,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="560" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="560" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A560" t="s">
         <v>1894</v>
       </c>
@@ -42158,7 +42164,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="571" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="571" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A571" t="s">
         <v>1918</v>
       </c>
@@ -42218,7 +42224,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="572" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="572" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A572" t="s">
         <v>1921</v>
       </c>
@@ -42278,7 +42284,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="573" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="573" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A573" t="s">
         <v>1922</v>
       </c>
@@ -42338,7 +42344,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="574" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="574" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A574" t="s">
         <v>1925</v>
       </c>
@@ -42398,7 +42404,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="575" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="575" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A575" t="s">
         <v>1928</v>
       </c>
@@ -42458,7 +42464,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="576" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="576" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A576" t="s">
         <v>1931</v>
       </c>
@@ -42518,7 +42524,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="577" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="577" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A577" t="s">
         <v>1934</v>
       </c>
@@ -42578,7 +42584,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="578" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="578" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A578" t="s">
         <v>1937</v>
       </c>
@@ -42638,7 +42644,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="579" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="579" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A579" t="s">
         <v>1941</v>
       </c>
@@ -42698,7 +42704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="580" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="580" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A580" t="s">
         <v>1945</v>
       </c>
@@ -42758,7 +42764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="581" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="581" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A581" t="s">
         <v>1948</v>
       </c>
@@ -42818,7 +42824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="582" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="582" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A582" t="s">
         <v>1951</v>
       </c>
@@ -42878,7 +42884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="583" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="583" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A583" t="s">
         <v>1954</v>
       </c>
@@ -42938,7 +42944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="584" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="584" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A584" t="s">
         <v>1957</v>
       </c>
@@ -42998,7 +43004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="585" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="585" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A585" t="s">
         <v>1960</v>
       </c>
@@ -43058,7 +43064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="586" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="586" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A586" t="s">
         <v>1963</v>
       </c>
@@ -43118,7 +43124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="587" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="587" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A587" t="s">
         <v>1966</v>
       </c>
@@ -43178,7 +43184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="588" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="588" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A588" t="s">
         <v>1969</v>
       </c>
@@ -43238,7 +43244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="589" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="589" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A589" t="s">
         <v>1972</v>
       </c>
@@ -43298,7 +43304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="590" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="590" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A590" t="s">
         <v>1976</v>
       </c>
@@ -43358,7 +43364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="591" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="591" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A591" t="s">
         <v>1980</v>
       </c>
@@ -43418,7 +43424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="592" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="592" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A592" t="s">
         <v>1984</v>
       </c>
@@ -43478,7 +43484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="593" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="593" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A593" t="s">
         <v>1987</v>
       </c>
@@ -43538,7 +43544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="594" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="594" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A594" t="s">
         <v>1990</v>
       </c>
@@ -43598,7 +43604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="595" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="595" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A595" t="s">
         <v>1993</v>
       </c>
@@ -43658,7 +43664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="596" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="596" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A596" t="s">
         <v>1996</v>
       </c>
@@ -43718,7 +43724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="597" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="597" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A597" t="s">
         <v>1999</v>
       </c>
@@ -43778,7 +43784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="598" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="598" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A598" t="s">
         <v>2002</v>
       </c>
@@ -43838,7 +43844,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="599" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="599" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A599" t="s">
         <v>2007</v>
       </c>
@@ -43898,7 +43904,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="600" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="600" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A600" t="s">
         <v>2011</v>
       </c>
@@ -43958,7 +43964,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="601" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="601" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A601" t="s">
         <v>2014</v>
       </c>
@@ -44018,7 +44024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="602" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="602" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A602" t="s">
         <v>2018</v>
       </c>
@@ -44078,7 +44084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="603" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="603" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A603" t="s">
         <v>2021</v>
       </c>
@@ -44138,7 +44144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="604" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="604" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A604" t="s">
         <v>2024</v>
       </c>
@@ -44198,7 +44204,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="605" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="605" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A605" t="s">
         <v>2027</v>
       </c>
@@ -44258,7 +44264,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="606" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="606" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A606" t="s">
         <v>2030</v>
       </c>
@@ -44318,7 +44324,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="607" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="607" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A607" t="s">
         <v>2033</v>
       </c>
@@ -44378,7 +44384,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="608" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="608" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A608" t="s">
         <v>2036</v>
       </c>
@@ -44438,7 +44444,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="609" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="609" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A609" t="s">
         <v>2039</v>
       </c>
@@ -44498,7 +44504,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="610" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="610" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A610" t="s">
         <v>2042</v>
       </c>
@@ -44558,7 +44564,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="611" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="611" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A611" t="s">
         <v>2045</v>
       </c>
@@ -44618,7 +44624,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="612" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="612" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A612" t="s">
         <v>2047</v>
       </c>
@@ -44678,7 +44684,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="613" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="613" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A613" t="s">
         <v>2050</v>
       </c>
@@ -44738,7 +44744,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="614" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="614" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A614" t="s">
         <v>2053</v>
       </c>
@@ -44798,7 +44804,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="615" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="615" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A615" t="s">
         <v>2056</v>
       </c>
@@ -44858,7 +44864,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="616" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="616" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A616" t="s">
         <v>2059</v>
       </c>
@@ -45158,7 +45164,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="621" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="621" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A621" t="s">
         <v>2072</v>
       </c>
@@ -45218,7 +45224,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="622" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="622" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A622" t="s">
         <v>2075</v>
       </c>
@@ -45278,7 +45284,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="623" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="623" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A623" t="s">
         <v>2078</v>
       </c>
@@ -45338,7 +45344,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="624" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="624" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A624" t="s">
         <v>2081</v>
       </c>
@@ -45398,7 +45404,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="625" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="625" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A625" t="s">
         <v>2084</v>
       </c>
@@ -45458,7 +45464,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="626" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="626" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A626" t="s">
         <v>2087</v>
       </c>
@@ -45518,7 +45524,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="627" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="627" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A627" t="s">
         <v>2090</v>
       </c>
@@ -45578,7 +45584,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="628" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="628" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A628" t="s">
         <v>2093</v>
       </c>
@@ -45638,7 +45644,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="629" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="629" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A629" t="s">
         <v>2096</v>
       </c>
@@ -45698,7 +45704,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="630" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="630" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A630" t="s">
         <v>2099</v>
       </c>
@@ -45758,7 +45764,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="631" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="631" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A631" t="s">
         <v>2102</v>
       </c>
@@ -45818,7 +45824,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="632" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="632" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A632" t="s">
         <v>2105</v>
       </c>
@@ -45878,7 +45884,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="633" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="633" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A633" t="s">
         <v>2108</v>
       </c>
@@ -45938,7 +45944,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="634" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="634" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A634" t="s">
         <v>2111</v>
       </c>
@@ -45998,7 +46004,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="635" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="635" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A635" t="s">
         <v>2114</v>
       </c>
@@ -46058,7 +46064,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="636" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="636" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A636" t="s">
         <v>2117</v>
       </c>
@@ -46118,7 +46124,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="637" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="637" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A637" t="s">
         <v>2120</v>
       </c>
@@ -46178,7 +46184,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="638" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="638" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A638" t="s">
         <v>2123</v>
       </c>
@@ -46238,7 +46244,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="639" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="639" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A639" t="s">
         <v>2126</v>
       </c>
@@ -46298,7 +46304,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="640" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="640" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A640" t="s">
         <v>2129</v>
       </c>
@@ -46358,7 +46364,7 @@
         <v>11f4</v>
       </c>
     </row>
-    <row r="641" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="641" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A641" t="s">
         <v>2132</v>
       </c>
@@ -46418,7 +46424,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="642" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="642" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A642" t="s">
         <v>2135</v>
       </c>
@@ -46478,7 +46484,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="643" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="643" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A643" t="s">
         <v>2138</v>
       </c>
@@ -46538,7 +46544,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="644" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="644" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A644" t="s">
         <v>2141</v>
       </c>
@@ -46598,7 +46604,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="645" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="645" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A645" t="s">
         <v>2144</v>
       </c>
@@ -46658,7 +46664,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="646" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="646" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A646" t="s">
         <v>2147</v>
       </c>
@@ -46718,7 +46724,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="647" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="647" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A647" t="s">
         <v>2150</v>
       </c>
@@ -46778,7 +46784,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="648" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="648" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A648" t="s">
         <v>2152</v>
       </c>

</xml_diff>

<commit_message>
Finished fixes after the 2024-02-12 meeting. TODO: test run.
</commit_message>
<xml_diff>
--- a/JAF_indicators__definitions.xlsx
+++ b/JAF_indicators__definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/JAF2R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="11_8EB80073D8E76818760C99562770445F322C70A0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{491490BB-75BF-4589-B1E9-1636ABB3AB2F}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="11_8EB80073D8E76818760C99562770445F322C70A0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{448F8D0E-C830-45CA-A944-7D76A650FE3C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7662,13 +7662,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="jaf" displayName="jaf" ref="A2:J648" totalsRowShown="0">
-  <autoFilter ref="A2:J648" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:J648" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="JAF_KEY"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -8084,7 +8078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -8144,7 +8138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -8204,7 +8198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -8264,7 +8258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -8324,7 +8318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -8384,7 +8378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -8444,7 +8438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -8504,7 +8498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -8564,7 +8558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -8624,7 +8618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -8684,7 +8678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -8744,7 +8738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -8804,7 +8798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -8864,7 +8858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -8924,7 +8918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -8984,7 +8978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -9044,7 +9038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -9104,7 +9098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -9164,7 +9158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -9224,7 +9218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -9284,7 +9278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -9344,7 +9338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -9404,7 +9398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -9464,7 +9458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -9524,7 +9518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -9584,7 +9578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -9644,7 +9638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -9704,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -9764,7 +9758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>141</v>
       </c>
@@ -9824,7 +9818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -9884,7 +9878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -9944,7 +9938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -10004,7 +9998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -10064,7 +10058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -10124,7 +10118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -10184,7 +10178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -10244,7 +10238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>173</v>
       </c>
@@ -10304,7 +10298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>177</v>
       </c>
@@ -10364,7 +10358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -10424,7 +10418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>185</v>
       </c>
@@ -10484,7 +10478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>189</v>
       </c>
@@ -10544,7 +10538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>193</v>
       </c>
@@ -10604,7 +10598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>197</v>
       </c>
@@ -10664,7 +10658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>201</v>
       </c>
@@ -10724,7 +10718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>205</v>
       </c>
@@ -10784,7 +10778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -10844,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>213</v>
       </c>
@@ -10904,7 +10898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>217</v>
       </c>
@@ -10964,7 +10958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -11024,7 +11018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -11084,7 +11078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -11144,7 +11138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>232</v>
       </c>
@@ -11204,7 +11198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>236</v>
       </c>
@@ -11264,7 +11258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -11324,7 +11318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>245</v>
       </c>
@@ -11384,7 +11378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -11444,7 +11438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>251</v>
       </c>
@@ -11504,7 +11498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>254</v>
       </c>
@@ -11564,7 +11558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>257</v>
       </c>
@@ -11624,7 +11618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>260</v>
       </c>
@@ -11684,7 +11678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>263</v>
       </c>
@@ -11744,7 +11738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>266</v>
       </c>
@@ -11804,7 +11798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>269</v>
       </c>
@@ -11864,7 +11858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>272</v>
       </c>
@@ -11924,7 +11918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>275</v>
       </c>
@@ -11984,7 +11978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>278</v>
       </c>
@@ -12044,7 +12038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>281</v>
       </c>
@@ -12104,7 +12098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>284</v>
       </c>
@@ -12164,7 +12158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -12224,7 +12218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>290</v>
       </c>
@@ -12284,7 +12278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>293</v>
       </c>
@@ -12344,7 +12338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>296</v>
       </c>
@@ -12404,7 +12398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>299</v>
       </c>
@@ -12464,7 +12458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>303</v>
       </c>
@@ -12524,7 +12518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>307</v>
       </c>
@@ -12584,7 +12578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>311</v>
       </c>
@@ -12644,7 +12638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>315</v>
       </c>
@@ -12704,7 +12698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>319</v>
       </c>
@@ -12764,7 +12758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>323</v>
       </c>
@@ -12824,7 +12818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>326</v>
       </c>
@@ -12884,7 +12878,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>329</v>
       </c>
@@ -12944,7 +12938,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>333</v>
       </c>
@@ -13004,7 +12998,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>337</v>
       </c>
@@ -13064,7 +13058,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>340</v>
       </c>
@@ -13124,7 +13118,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>344</v>
       </c>
@@ -13184,7 +13178,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>348</v>
       </c>
@@ -13244,7 +13238,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>351</v>
       </c>
@@ -13304,7 +13298,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>354</v>
       </c>
@@ -13364,7 +13358,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>359</v>
       </c>
@@ -13424,7 +13418,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>362</v>
       </c>
@@ -13484,7 +13478,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>365</v>
       </c>
@@ -13544,7 +13538,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>368</v>
       </c>
@@ -13604,7 +13598,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>371</v>
       </c>
@@ -13664,7 +13658,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>375</v>
       </c>
@@ -13724,7 +13718,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>378</v>
       </c>
@@ -13784,7 +13778,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>381</v>
       </c>
@@ -13844,7 +13838,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>385</v>
       </c>
@@ -13904,7 +13898,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>389</v>
       </c>
@@ -13964,7 +13958,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>393</v>
       </c>
@@ -14024,7 +14018,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>397</v>
       </c>
@@ -14084,7 +14078,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>401</v>
       </c>
@@ -14144,7 +14138,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>405</v>
       </c>
@@ -14204,7 +14198,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>409</v>
       </c>
@@ -14264,7 +14258,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>413</v>
       </c>
@@ -14324,7 +14318,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>417</v>
       </c>
@@ -14384,7 +14378,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>421</v>
       </c>
@@ -14444,7 +14438,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>425</v>
       </c>
@@ -14504,7 +14498,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>429</v>
       </c>
@@ -14564,7 +14558,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>432</v>
       </c>
@@ -14624,7 +14618,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>435</v>
       </c>
@@ -14684,7 +14678,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>438</v>
       </c>
@@ -14744,7 +14738,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>441</v>
       </c>
@@ -14804,7 +14798,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>444</v>
       </c>
@@ -14864,7 +14858,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>447</v>
       </c>
@@ -14924,7 +14918,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>450</v>
       </c>
@@ -14984,7 +14978,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>453</v>
       </c>
@@ -15044,7 +15038,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>457</v>
       </c>
@@ -15104,7 +15098,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>460</v>
       </c>
@@ -15164,7 +15158,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>463</v>
       </c>
@@ -15224,7 +15218,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="122" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>466</v>
       </c>
@@ -15284,7 +15278,7 @@
         <v>1b</v>
       </c>
     </row>
-    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>467</v>
       </c>
@@ -15344,7 +15338,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>469</v>
       </c>
@@ -15404,7 +15398,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>473</v>
       </c>
@@ -15464,7 +15458,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>477</v>
       </c>
@@ -15524,7 +15518,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>481</v>
       </c>
@@ -15584,7 +15578,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>482</v>
       </c>
@@ -15644,7 +15638,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>487</v>
       </c>
@@ -15704,7 +15698,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>490</v>
       </c>
@@ -15764,7 +15758,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>493</v>
       </c>
@@ -15824,7 +15818,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>496</v>
       </c>
@@ -15884,7 +15878,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>500</v>
       </c>
@@ -15944,7 +15938,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>504</v>
       </c>
@@ -16004,7 +15998,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>508</v>
       </c>
@@ -16064,7 +16058,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>513</v>
       </c>
@@ -16124,7 +16118,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>517</v>
       </c>
@@ -16184,7 +16178,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>520</v>
       </c>
@@ -16244,7 +16238,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>524</v>
       </c>
@@ -16304,7 +16298,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>527</v>
       </c>
@@ -16364,7 +16358,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>531</v>
       </c>
@@ -16424,7 +16418,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>534</v>
       </c>
@@ -16484,7 +16478,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>537</v>
       </c>
@@ -16544,7 +16538,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>541</v>
       </c>
@@ -16604,7 +16598,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>545</v>
       </c>
@@ -16664,7 +16658,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>549</v>
       </c>
@@ -16724,7 +16718,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>553</v>
       </c>
@@ -16784,7 +16778,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>557</v>
       </c>
@@ -16844,7 +16838,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>561</v>
       </c>
@@ -16904,7 +16898,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>562</v>
       </c>
@@ -16964,7 +16958,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>566</v>
       </c>
@@ -17024,7 +17018,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>567</v>
       </c>
@@ -17084,7 +17078,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>570</v>
       </c>
@@ -17144,7 +17138,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>573</v>
       </c>
@@ -17204,7 +17198,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>576</v>
       </c>
@@ -17264,7 +17258,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>580</v>
       </c>
@@ -17324,7 +17318,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>584</v>
       </c>
@@ -17384,7 +17378,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>588</v>
       </c>
@@ -17444,7 +17438,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>591</v>
       </c>
@@ -17504,7 +17498,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>595</v>
       </c>
@@ -17564,7 +17558,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>598</v>
       </c>
@@ -17624,7 +17618,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>601</v>
       </c>
@@ -17684,7 +17678,7 @@
         <v>1c</v>
       </c>
     </row>
-    <row r="163" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>604</v>
       </c>
@@ -17744,7 +17738,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>606</v>
       </c>
@@ -17804,7 +17798,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>610</v>
       </c>
@@ -17864,7 +17858,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>614</v>
       </c>
@@ -17924,7 +17918,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>618</v>
       </c>
@@ -17984,7 +17978,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>622</v>
       </c>
@@ -18044,7 +18038,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>626</v>
       </c>
@@ -18104,7 +18098,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>630</v>
       </c>
@@ -18164,7 +18158,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>634</v>
       </c>
@@ -18224,7 +18218,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>638</v>
       </c>
@@ -18284,7 +18278,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>642</v>
       </c>
@@ -18344,7 +18338,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>646</v>
       </c>
@@ -18404,7 +18398,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>650</v>
       </c>
@@ -18464,7 +18458,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>653</v>
       </c>
@@ -18524,7 +18518,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>656</v>
       </c>
@@ -18584,7 +18578,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>659</v>
       </c>
@@ -18644,7 +18638,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>662</v>
       </c>
@@ -18704,7 +18698,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>665</v>
       </c>
@@ -18764,7 +18758,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>668</v>
       </c>
@@ -18824,7 +18818,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="182" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>672</v>
       </c>
@@ -18884,7 +18878,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="183" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>676</v>
       </c>
@@ -18944,7 +18938,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>680</v>
       </c>
@@ -19004,7 +18998,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="185" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>684</v>
       </c>
@@ -19064,7 +19058,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="186" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>688</v>
       </c>
@@ -19124,7 +19118,7 @@
         <v>1d</v>
       </c>
     </row>
-    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>692</v>
       </c>
@@ -19184,7 +19178,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>697</v>
       </c>
@@ -19244,7 +19238,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="189" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>702</v>
       </c>
@@ -19304,7 +19298,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="190" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>706</v>
       </c>
@@ -19364,7 +19358,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="191" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>710</v>
       </c>
@@ -19424,7 +19418,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="192" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>714</v>
       </c>
@@ -19484,7 +19478,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="193" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>718</v>
       </c>
@@ -19544,7 +19538,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="194" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>721</v>
       </c>
@@ -19604,7 +19598,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="195" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>725</v>
       </c>
@@ -19664,7 +19658,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="196" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>729</v>
       </c>
@@ -19724,7 +19718,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>733</v>
       </c>
@@ -19784,7 +19778,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="198" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>737</v>
       </c>
@@ -19844,7 +19838,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="199" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>741</v>
       </c>
@@ -19904,7 +19898,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="200" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>745</v>
       </c>
@@ -19964,7 +19958,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="201" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>751</v>
       </c>
@@ -20024,7 +20018,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="202" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>757</v>
       </c>
@@ -20084,7 +20078,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="203" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>760</v>
       </c>
@@ -20144,7 +20138,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>764</v>
       </c>
@@ -20204,7 +20198,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="205" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>768</v>
       </c>
@@ -20264,7 +20258,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="206" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>771</v>
       </c>
@@ -20324,7 +20318,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="207" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>775</v>
       </c>
@@ -20384,7 +20378,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="208" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>779</v>
       </c>
@@ -20444,7 +20438,7 @@
         <v>2a</v>
       </c>
     </row>
-    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>783</v>
       </c>
@@ -20504,7 +20498,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>787</v>
       </c>
@@ -20564,7 +20558,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>791</v>
       </c>
@@ -20624,7 +20618,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="212" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>795</v>
       </c>
@@ -20684,7 +20678,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="213" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>798</v>
       </c>
@@ -20744,7 +20738,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>802</v>
       </c>
@@ -20804,7 +20798,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="215" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>805</v>
       </c>
@@ -20864,7 +20858,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>808</v>
       </c>
@@ -20924,7 +20918,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>811</v>
       </c>
@@ -20984,7 +20978,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>815</v>
       </c>
@@ -21044,7 +21038,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>818</v>
       </c>
@@ -21104,7 +21098,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>822</v>
       </c>
@@ -21164,7 +21158,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="221" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>826</v>
       </c>
@@ -21224,7 +21218,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>827</v>
       </c>
@@ -21284,7 +21278,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>829</v>
       </c>
@@ -21344,7 +21338,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="224" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>833</v>
       </c>
@@ -21404,7 +21398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>835</v>
       </c>
@@ -21464,7 +21458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>839</v>
       </c>
@@ -21584,7 +21578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>848</v>
       </c>
@@ -21644,7 +21638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>852</v>
       </c>
@@ -21704,7 +21698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>856</v>
       </c>
@@ -21764,7 +21758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>861</v>
       </c>
@@ -21824,7 +21818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>864</v>
       </c>
@@ -21884,7 +21878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>867</v>
       </c>
@@ -21944,7 +21938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>870</v>
       </c>
@@ -22004,7 +21998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>873</v>
       </c>
@@ -22064,7 +22058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>876</v>
       </c>
@@ -22124,7 +22118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>879</v>
       </c>
@@ -22244,7 +22238,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="239" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>886</v>
       </c>
@@ -22304,7 +22298,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="240" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>889</v>
       </c>
@@ -22364,7 +22358,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="241" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>894</v>
       </c>
@@ -22424,7 +22418,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="242" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>897</v>
       </c>
@@ -22484,7 +22478,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="243" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>900</v>
       </c>
@@ -22544,7 +22538,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="244" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>903</v>
       </c>
@@ -22604,7 +22598,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="245" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>906</v>
       </c>
@@ -22664,7 +22658,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="246" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>909</v>
       </c>
@@ -22724,7 +22718,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="247" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>912</v>
       </c>
@@ -22784,7 +22778,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="248" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>915</v>
       </c>
@@ -22844,7 +22838,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="249" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>919</v>
       </c>
@@ -22904,7 +22898,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="250" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>922</v>
       </c>
@@ -22964,7 +22958,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="251" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>925</v>
       </c>
@@ -23084,7 +23078,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="253" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>934</v>
       </c>
@@ -23144,7 +23138,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="254" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>939</v>
       </c>
@@ -23204,7 +23198,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="255" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>943</v>
       </c>
@@ -23264,7 +23258,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>946</v>
       </c>
@@ -23324,7 +23318,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="257" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>949</v>
       </c>
@@ -23384,7 +23378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>953</v>
       </c>
@@ -23444,7 +23438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>957</v>
       </c>
@@ -23504,7 +23498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>960</v>
       </c>
@@ -23564,7 +23558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>963</v>
       </c>
@@ -23624,7 +23618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>966</v>
       </c>
@@ -23684,7 +23678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>970</v>
       </c>
@@ -23744,7 +23738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>975</v>
       </c>
@@ -23804,7 +23798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>978</v>
       </c>
@@ -23864,7 +23858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>981</v>
       </c>
@@ -23924,7 +23918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>984</v>
       </c>
@@ -23984,7 +23978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>987</v>
       </c>
@@ -24044,7 +24038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>990</v>
       </c>
@@ -24104,7 +24098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>993</v>
       </c>
@@ -24164,7 +24158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>997</v>
       </c>
@@ -24224,7 +24218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>1001</v>
       </c>
@@ -24284,7 +24278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>1004</v>
       </c>
@@ -24344,7 +24338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>1007</v>
       </c>
@@ -24404,7 +24398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>1010</v>
       </c>
@@ -24464,7 +24458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>1014</v>
       </c>
@@ -25064,7 +25058,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="286" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>1048</v>
       </c>
@@ -25124,7 +25118,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="287" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>1052</v>
       </c>
@@ -25184,7 +25178,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="288" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>1057</v>
       </c>
@@ -25244,7 +25238,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="289" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>1060</v>
       </c>
@@ -25304,7 +25298,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="290" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>1063</v>
       </c>
@@ -25364,7 +25358,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>1066</v>
       </c>
@@ -25424,7 +25418,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>1069</v>
       </c>
@@ -25484,7 +25478,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>1072</v>
       </c>
@@ -25544,7 +25538,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="294" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>1075</v>
       </c>
@@ -25604,7 +25598,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="295" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>1078</v>
       </c>
@@ -25664,7 +25658,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="296" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>1082</v>
       </c>
@@ -25724,7 +25718,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="297" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>1086</v>
       </c>
@@ -25784,7 +25778,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="298" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>1090</v>
       </c>
@@ -25844,7 +25838,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="299" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>1094</v>
       </c>
@@ -25904,7 +25898,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>1097</v>
       </c>
@@ -25964,7 +25958,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>1102</v>
       </c>
@@ -26024,7 +26018,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="302" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>1107</v>
       </c>
@@ -26084,7 +26078,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="303" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>1111</v>
       </c>
@@ -26204,7 +26198,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="305" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>1116</v>
       </c>
@@ -26264,7 +26258,7 @@
         <v>6b</v>
       </c>
     </row>
-    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>1120</v>
       </c>
@@ -26324,7 +26318,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>1125</v>
       </c>
@@ -26384,7 +26378,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>1130</v>
       </c>
@@ -26444,7 +26438,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>1134</v>
       </c>
@@ -26504,7 +26498,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="310" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
         <v>1138</v>
       </c>
@@ -26564,7 +26558,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="311" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>1142</v>
       </c>
@@ -26624,7 +26618,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="312" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>1146</v>
       </c>
@@ -26684,7 +26678,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="313" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>1150</v>
       </c>
@@ -26744,7 +26738,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="314" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>1152</v>
       </c>
@@ -26804,7 +26798,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>1154</v>
       </c>
@@ -26864,7 +26858,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>1158</v>
       </c>
@@ -26924,7 +26918,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="317" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>1163</v>
       </c>
@@ -26984,7 +26978,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="318" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>1165</v>
       </c>
@@ -27044,7 +27038,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="319" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>1169</v>
       </c>
@@ -27104,7 +27098,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="320" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>1172</v>
       </c>
@@ -27164,7 +27158,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="321" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>1175</v>
       </c>
@@ -27224,7 +27218,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A322" t="s">
         <v>1180</v>
       </c>
@@ -27284,7 +27278,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>1181</v>
       </c>
@@ -27344,7 +27338,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A324" t="s">
         <v>1184</v>
       </c>
@@ -27404,7 +27398,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>1187</v>
       </c>
@@ -27464,7 +27458,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A326" t="s">
         <v>1190</v>
       </c>
@@ -27524,7 +27518,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>1193</v>
       </c>
@@ -27584,7 +27578,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A328" t="s">
         <v>1194</v>
       </c>
@@ -27644,7 +27638,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>1195</v>
       </c>
@@ -27704,7 +27698,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A330" t="s">
         <v>1196</v>
       </c>
@@ -27764,7 +27758,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>1197</v>
       </c>
@@ -27824,7 +27818,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>1202</v>
       </c>
@@ -27884,7 +27878,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>1206</v>
       </c>
@@ -27944,7 +27938,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A334" t="s">
         <v>1209</v>
       </c>
@@ -28004,7 +27998,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>1213</v>
       </c>
@@ -28124,7 +28118,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>1223</v>
       </c>
@@ -28184,7 +28178,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A338" t="s">
         <v>1228</v>
       </c>
@@ -28244,7 +28238,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>1231</v>
       </c>
@@ -28304,7 +28298,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
         <v>1236</v>
       </c>
@@ -28364,7 +28358,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>1239</v>
       </c>
@@ -28424,7 +28418,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>1243</v>
       </c>
@@ -28484,7 +28478,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>1247</v>
       </c>
@@ -28544,7 +28538,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>1251</v>
       </c>
@@ -28604,7 +28598,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>1256</v>
       </c>
@@ -28664,7 +28658,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>1260</v>
       </c>
@@ -28724,7 +28718,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>1264</v>
       </c>
@@ -28784,7 +28778,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>1268</v>
       </c>
@@ -28844,7 +28838,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>1272</v>
       </c>
@@ -28904,7 +28898,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>1276</v>
       </c>
@@ -28964,7 +28958,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>1280</v>
       </c>
@@ -29024,7 +29018,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>1285</v>
       </c>
@@ -29084,7 +29078,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>1289</v>
       </c>
@@ -29144,7 +29138,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A354" t="s">
         <v>1293</v>
       </c>
@@ -29204,7 +29198,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>1297</v>
       </c>
@@ -29264,7 +29258,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
         <v>1300</v>
       </c>
@@ -29324,7 +29318,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>1304</v>
       </c>
@@ -29384,7 +29378,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>1308</v>
       </c>
@@ -29444,7 +29438,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>1312</v>
       </c>
@@ -29504,7 +29498,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A360" t="s">
         <v>1316</v>
       </c>
@@ -29564,7 +29558,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>1320</v>
       </c>
@@ -29624,7 +29618,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>1324</v>
       </c>
@@ -29684,7 +29678,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>1327</v>
       </c>
@@ -29744,7 +29738,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
         <v>1330</v>
       </c>
@@ -29804,7 +29798,7 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A365" t="s">
         <v>1332</v>
       </c>
@@ -29864,7 +29858,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A366" t="s">
         <v>1337</v>
       </c>
@@ -29924,7 +29918,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
         <v>1341</v>
       </c>
@@ -29984,7 +29978,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A368" t="s">
         <v>1343</v>
       </c>
@@ -30044,7 +30038,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A369" t="s">
         <v>1345</v>
       </c>
@@ -30104,7 +30098,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="370" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A370" t="s">
         <v>1348</v>
       </c>
@@ -30164,7 +30158,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A371" t="s">
         <v>1351</v>
       </c>
@@ -30224,7 +30218,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A372" t="s">
         <v>1355</v>
       </c>
@@ -30284,7 +30278,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A373" t="s">
         <v>1359</v>
       </c>
@@ -30344,7 +30338,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A374" t="s">
         <v>1363</v>
       </c>
@@ -30404,7 +30398,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A375" t="s">
         <v>1367</v>
       </c>
@@ -30464,7 +30458,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A376" t="s">
         <v>1370</v>
       </c>
@@ -30524,7 +30518,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A377" t="s">
         <v>1374</v>
       </c>
@@ -30584,7 +30578,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A378" t="s">
         <v>1378</v>
       </c>
@@ -30644,7 +30638,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A379" t="s">
         <v>1382</v>
       </c>
@@ -30704,7 +30698,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="380" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A380" t="s">
         <v>1386</v>
       </c>
@@ -30764,7 +30758,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="381" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A381" t="s">
         <v>1388</v>
       </c>
@@ -30824,7 +30818,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="382" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A382" t="s">
         <v>1390</v>
       </c>
@@ -30884,7 +30878,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="383" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
         <v>1392</v>
       </c>
@@ -30944,7 +30938,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="384" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A384" t="s">
         <v>1394</v>
       </c>
@@ -31004,7 +30998,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="385" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>1397</v>
       </c>
@@ -31064,7 +31058,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="386" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A386" t="s">
         <v>1400</v>
       </c>
@@ -31124,7 +31118,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="387" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A387" t="s">
         <v>1403</v>
       </c>
@@ -31184,7 +31178,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="388" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A388" t="s">
         <v>1406</v>
       </c>
@@ -31244,7 +31238,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="389" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A389" t="s">
         <v>1411</v>
       </c>
@@ -31304,7 +31298,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="390" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A390" t="s">
         <v>1416</v>
       </c>
@@ -31364,7 +31358,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="391" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A391" t="s">
         <v>1419</v>
       </c>
@@ -31424,7 +31418,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="392" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A392" t="s">
         <v>1422</v>
       </c>
@@ -31484,7 +31478,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="393" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A393" t="s">
         <v>1425</v>
       </c>
@@ -31544,7 +31538,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="394" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A394" t="s">
         <v>1428</v>
       </c>
@@ -31604,7 +31598,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="395" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>1431</v>
       </c>
@@ -31664,7 +31658,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="396" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A396" t="s">
         <v>1435</v>
       </c>
@@ -31724,7 +31718,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="397" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A397" t="s">
         <v>1439</v>
       </c>
@@ -31784,7 +31778,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="398" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A398" t="s">
         <v>1443</v>
       </c>
@@ -31844,7 +31838,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="399" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
         <v>1447</v>
       </c>
@@ -31904,7 +31898,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="400" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A400" t="s">
         <v>1450</v>
       </c>
@@ -31964,7 +31958,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="401" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A401" t="s">
         <v>1453</v>
       </c>
@@ -32024,7 +32018,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="402" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A402" t="s">
         <v>1456</v>
       </c>
@@ -32084,7 +32078,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="403" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A403" t="s">
         <v>1459</v>
       </c>
@@ -32144,7 +32138,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="404" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A404" t="s">
         <v>1462</v>
       </c>
@@ -32204,7 +32198,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="405" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A405" t="s">
         <v>1465</v>
       </c>
@@ -32264,7 +32258,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="406" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A406" t="s">
         <v>1468</v>
       </c>
@@ -32324,7 +32318,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="407" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A407" t="s">
         <v>1472</v>
       </c>
@@ -32384,7 +32378,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="408" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A408" t="s">
         <v>1475</v>
       </c>
@@ -32624,7 +32618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="412" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A412" t="s">
         <v>1485</v>
       </c>
@@ -32684,7 +32678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="413" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A413" t="s">
         <v>1488</v>
       </c>
@@ -33224,7 +33218,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="422" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A422" t="s">
         <v>1514</v>
       </c>
@@ -33284,7 +33278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="423" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A423" t="s">
         <v>1517</v>
       </c>
@@ -33344,7 +33338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="424" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A424" t="s">
         <v>1519</v>
       </c>
@@ -33404,7 +33398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="425" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A425" t="s">
         <v>1522</v>
       </c>
@@ -33464,7 +33458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="426" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A426" t="s">
         <v>1525</v>
       </c>
@@ -33524,7 +33518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="427" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A427" t="s">
         <v>1530</v>
       </c>
@@ -33584,7 +33578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="428" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A428" t="s">
         <v>1532</v>
       </c>
@@ -33644,7 +33638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="429" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A429" t="s">
         <v>1536</v>
       </c>
@@ -33704,7 +33698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="430" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A430" t="s">
         <v>1537</v>
       </c>
@@ -33764,7 +33758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="431" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A431" t="s">
         <v>1540</v>
       </c>
@@ -34784,7 +34778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="448" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A448" t="s">
         <v>1587</v>
       </c>
@@ -34844,7 +34838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="449" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A449" t="s">
         <v>1590</v>
       </c>
@@ -34964,7 +34958,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="451" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A451" t="s">
         <v>1594</v>
       </c>
@@ -35024,7 +35018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="452" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A452" t="s">
         <v>1597</v>
       </c>
@@ -35084,7 +35078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="453" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A453" t="s">
         <v>1598</v>
       </c>
@@ -35204,7 +35198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="455" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A455" t="s">
         <v>1605</v>
       </c>
@@ -35264,7 +35258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="456" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A456" t="s">
         <v>1610</v>
       </c>
@@ -35324,7 +35318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="457" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A457" t="s">
         <v>1614</v>
       </c>
@@ -35384,7 +35378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="458" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A458" t="s">
         <v>1618</v>
       </c>
@@ -35444,7 +35438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="459" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A459" t="s">
         <v>1623</v>
       </c>
@@ -35504,7 +35498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="460" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A460" t="s">
         <v>1626</v>
       </c>
@@ -35564,7 +35558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="461" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A461" t="s">
         <v>1629</v>
       </c>
@@ -35624,7 +35618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="462" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A462" t="s">
         <v>1632</v>
       </c>
@@ -35684,7 +35678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="463" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A463" t="s">
         <v>1635</v>
       </c>
@@ -35744,7 +35738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="464" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A464" t="s">
         <v>1638</v>
       </c>
@@ -35804,7 +35798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="465" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A465" t="s">
         <v>1641</v>
       </c>
@@ -35864,7 +35858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="466" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A466" t="s">
         <v>1644</v>
       </c>
@@ -35924,7 +35918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="467" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A467" t="s">
         <v>1647</v>
       </c>
@@ -35984,7 +35978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="468" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A468" t="s">
         <v>1650</v>
       </c>
@@ -36044,7 +36038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="469" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A469" t="s">
         <v>1653</v>
       </c>
@@ -36104,7 +36098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="470" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A470" t="s">
         <v>1656</v>
       </c>
@@ -36164,7 +36158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="471" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A471" t="s">
         <v>1659</v>
       </c>
@@ -36224,7 +36218,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="472" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="472" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A472" t="s">
         <v>1662</v>
       </c>
@@ -36284,7 +36278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="473" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A473" t="s">
         <v>1665</v>
       </c>
@@ -36344,7 +36338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="474" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="474" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A474" t="s">
         <v>1668</v>
       </c>
@@ -36404,7 +36398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="475" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="475" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A475" t="s">
         <v>1672</v>
       </c>
@@ -36464,7 +36458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="476" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="476" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A476" t="s">
         <v>1675</v>
       </c>
@@ -36524,7 +36518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="477" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="477" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A477" t="s">
         <v>1678</v>
       </c>
@@ -36584,7 +36578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="478" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="478" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A478" t="s">
         <v>1681</v>
       </c>
@@ -36644,7 +36638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="479" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A479" t="s">
         <v>1685</v>
       </c>
@@ -36704,7 +36698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="480" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="480" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A480" t="s">
         <v>1688</v>
       </c>
@@ -37004,7 +36998,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="485" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="485" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A485" t="s">
         <v>1702</v>
       </c>
@@ -37064,7 +37058,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="486" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="486" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A486" t="s">
         <v>1705</v>
       </c>
@@ -37124,7 +37118,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="487" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="487" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A487" t="s">
         <v>1708</v>
       </c>
@@ -37184,7 +37178,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="488" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="488" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A488" t="s">
         <v>1711</v>
       </c>
@@ -37724,7 +37718,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="497" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="497" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A497" t="s">
         <v>1732</v>
       </c>
@@ -37784,7 +37778,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="498" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="498" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A498" t="s">
         <v>1735</v>
       </c>
@@ -37964,7 +37958,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="501" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="501" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A501" t="s">
         <v>1742</v>
       </c>
@@ -38144,7 +38138,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="504" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="504" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A504" t="s">
         <v>1751</v>
       </c>
@@ -38204,7 +38198,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="505" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="505" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A505" t="s">
         <v>1754</v>
       </c>
@@ -38264,7 +38258,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="506" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="506" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A506" t="s">
         <v>1756</v>
       </c>
@@ -38324,7 +38318,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="507" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="507" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A507" t="s">
         <v>1759</v>
       </c>
@@ -38384,7 +38378,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="508" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="508" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A508" t="s">
         <v>1761</v>
       </c>
@@ -38444,7 +38438,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="509" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="509" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A509" t="s">
         <v>1765</v>
       </c>
@@ -38504,7 +38498,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="510" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="510" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A510" t="s">
         <v>1768</v>
       </c>
@@ -38804,7 +38798,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="515" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="515" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A515" t="s">
         <v>1781</v>
       </c>
@@ -38864,7 +38858,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="516" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="516" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A516" t="s">
         <v>1784</v>
       </c>
@@ -38924,7 +38918,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="517" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="517" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A517" t="s">
         <v>1787</v>
       </c>
@@ -38984,7 +38978,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="518" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="518" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A518" t="s">
         <v>1790</v>
       </c>
@@ -39044,7 +39038,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="519" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="519" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A519" t="s">
         <v>1794</v>
       </c>
@@ -39104,7 +39098,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="520" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="520" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A520" t="s">
         <v>1795</v>
       </c>
@@ -40004,7 +39998,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="535" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="535" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A535" t="s">
         <v>1829</v>
       </c>
@@ -40064,7 +40058,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="536" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="536" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A536" t="s">
         <v>1832</v>
       </c>
@@ -40124,7 +40118,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="537" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="537" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A537" t="s">
         <v>1833</v>
       </c>
@@ -40184,7 +40178,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="538" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="538" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A538" t="s">
         <v>1836</v>
       </c>
@@ -40244,7 +40238,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="539" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="539" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A539" t="s">
         <v>1839</v>
       </c>
@@ -40304,7 +40298,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="540" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="540" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A540" t="s">
         <v>1840</v>
       </c>
@@ -40364,7 +40358,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="541" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="541" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A541" t="s">
         <v>1842</v>
       </c>
@@ -40424,7 +40418,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="542" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="542" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A542" t="s">
         <v>1845</v>
       </c>
@@ -40484,7 +40478,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="543" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="543" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A543" t="s">
         <v>1848</v>
       </c>
@@ -40544,7 +40538,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="544" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="544" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A544" t="s">
         <v>1851</v>
       </c>
@@ -41204,7 +41198,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="555" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="555" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A555" t="s">
         <v>1879</v>
       </c>
@@ -41264,7 +41258,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="556" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="556" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A556" t="s">
         <v>1882</v>
       </c>
@@ -41324,7 +41318,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="557" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="557" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A557" t="s">
         <v>1885</v>
       </c>
@@ -41384,7 +41378,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="558" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="558" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A558" t="s">
         <v>1888</v>
       </c>
@@ -41444,7 +41438,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="559" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="559" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A559" t="s">
         <v>1891</v>
       </c>
@@ -41504,7 +41498,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="560" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="560" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A560" t="s">
         <v>1894</v>
       </c>
@@ -42164,7 +42158,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="571" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="571" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A571" t="s">
         <v>1918</v>
       </c>
@@ -42224,7 +42218,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="572" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="572" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A572" t="s">
         <v>1921</v>
       </c>
@@ -42284,7 +42278,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="573" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="573" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A573" t="s">
         <v>1922</v>
       </c>
@@ -42344,7 +42338,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="574" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="574" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A574" t="s">
         <v>1925</v>
       </c>
@@ -42404,7 +42398,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="575" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="575" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A575" t="s">
         <v>1928</v>
       </c>
@@ -42464,7 +42458,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="576" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="576" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A576" t="s">
         <v>1931</v>
       </c>
@@ -42524,7 +42518,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="577" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="577" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A577" t="s">
         <v>1934</v>
       </c>
@@ -42584,7 +42578,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="578" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="578" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A578" t="s">
         <v>1937</v>
       </c>
@@ -42644,7 +42638,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="579" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="579" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A579" t="s">
         <v>1941</v>
       </c>
@@ -42704,7 +42698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="580" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="580" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A580" t="s">
         <v>1945</v>
       </c>
@@ -42764,7 +42758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="581" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="581" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A581" t="s">
         <v>1948</v>
       </c>
@@ -42824,7 +42818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="582" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="582" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A582" t="s">
         <v>1951</v>
       </c>
@@ -42884,7 +42878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="583" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="583" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A583" t="s">
         <v>1954</v>
       </c>
@@ -42944,7 +42938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="584" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="584" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A584" t="s">
         <v>1957</v>
       </c>
@@ -43004,7 +42998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="585" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="585" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A585" t="s">
         <v>1960</v>
       </c>
@@ -43064,7 +43058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="586" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="586" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A586" t="s">
         <v>1963</v>
       </c>
@@ -43124,7 +43118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="587" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="587" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A587" t="s">
         <v>1966</v>
       </c>
@@ -43184,7 +43178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="588" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="588" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A588" t="s">
         <v>1969</v>
       </c>
@@ -43244,7 +43238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="589" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="589" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A589" t="s">
         <v>1972</v>
       </c>
@@ -43304,7 +43298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="590" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="590" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A590" t="s">
         <v>1976</v>
       </c>
@@ -43364,7 +43358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="591" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="591" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A591" t="s">
         <v>1980</v>
       </c>
@@ -43424,7 +43418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="592" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="592" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A592" t="s">
         <v>1984</v>
       </c>
@@ -43484,7 +43478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="593" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="593" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A593" t="s">
         <v>1987</v>
       </c>
@@ -43544,7 +43538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="594" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="594" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A594" t="s">
         <v>1990</v>
       </c>
@@ -43604,7 +43598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="595" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="595" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A595" t="s">
         <v>1993</v>
       </c>
@@ -43664,7 +43658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="596" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="596" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A596" t="s">
         <v>1996</v>
       </c>
@@ -43724,7 +43718,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="597" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="597" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A597" t="s">
         <v>1999</v>
       </c>
@@ -43784,7 +43778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="598" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="598" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A598" t="s">
         <v>2002</v>
       </c>
@@ -43844,7 +43838,7 @@
         <v>6a</v>
       </c>
     </row>
-    <row r="599" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="599" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A599" t="s">
         <v>2007</v>
       </c>
@@ -43904,7 +43898,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="600" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="600" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A600" t="s">
         <v>2011</v>
       </c>
@@ -43964,7 +43958,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row r="601" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="601" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A601" t="s">
         <v>2014</v>
       </c>
@@ -44024,7 +44018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="602" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="602" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A602" t="s">
         <v>2018</v>
       </c>
@@ -44084,7 +44078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="603" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="603" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A603" t="s">
         <v>2021</v>
       </c>
@@ -44144,7 +44138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="604" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="604" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A604" t="s">
         <v>2024</v>
       </c>
@@ -44204,7 +44198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="605" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="605" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A605" t="s">
         <v>2027</v>
       </c>
@@ -44264,7 +44258,7 @@
         <v>11a</v>
       </c>
     </row>
-    <row r="606" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="606" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A606" t="s">
         <v>2030</v>
       </c>
@@ -44324,7 +44318,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="607" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="607" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A607" t="s">
         <v>2033</v>
       </c>
@@ -44384,7 +44378,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="608" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="608" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A608" t="s">
         <v>2036</v>
       </c>
@@ -44444,7 +44438,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="609" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="609" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A609" t="s">
         <v>2039</v>
       </c>
@@ -44504,7 +44498,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="610" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="610" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A610" t="s">
         <v>2042</v>
       </c>
@@ -44564,7 +44558,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="611" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="611" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A611" t="s">
         <v>2045</v>
       </c>
@@ -44624,7 +44618,7 @@
         <v>11b</v>
       </c>
     </row>
-    <row r="612" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="612" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A612" t="s">
         <v>2047</v>
       </c>
@@ -44684,7 +44678,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="613" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="613" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A613" t="s">
         <v>2050</v>
       </c>
@@ -44744,7 +44738,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="614" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="614" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A614" t="s">
         <v>2053</v>
       </c>
@@ -44804,7 +44798,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="615" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="615" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A615" t="s">
         <v>2056</v>
       </c>
@@ -44864,7 +44858,7 @@
         <v>11c</v>
       </c>
     </row>
-    <row r="616" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="616" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A616" t="s">
         <v>2059</v>
       </c>
@@ -45164,7 +45158,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="621" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="621" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A621" t="s">
         <v>2072</v>
       </c>
@@ -45224,7 +45218,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="622" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="622" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A622" t="s">
         <v>2075</v>
       </c>
@@ -45284,7 +45278,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="623" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="623" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A623" t="s">
         <v>2078</v>
       </c>
@@ -45344,7 +45338,7 @@
         <v>11d1</v>
       </c>
     </row>
-    <row r="624" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="624" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A624" t="s">
         <v>2081</v>
       </c>
@@ -45404,7 +45398,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="625" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="625" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A625" t="s">
         <v>2084</v>
       </c>
@@ -45464,7 +45458,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="626" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="626" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A626" t="s">
         <v>2087</v>
       </c>
@@ -45524,7 +45518,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="627" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="627" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A627" t="s">
         <v>2090</v>
       </c>
@@ -45584,7 +45578,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="628" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="628" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A628" t="s">
         <v>2093</v>
       </c>
@@ -45644,7 +45638,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="629" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="629" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A629" t="s">
         <v>2096</v>
       </c>
@@ -45704,7 +45698,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="630" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="630" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A630" t="s">
         <v>2099</v>
       </c>
@@ -45764,7 +45758,7 @@
         <v>11f1</v>
       </c>
     </row>
-    <row r="631" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="631" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A631" t="s">
         <v>2102</v>
       </c>
@@ -45824,7 +45818,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="632" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="632" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A632" t="s">
         <v>2105</v>
       </c>
@@ -45884,7 +45878,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="633" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="633" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A633" t="s">
         <v>2108</v>
       </c>
@@ -45944,7 +45938,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="634" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="634" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A634" t="s">
         <v>2111</v>
       </c>
@@ -46004,7 +45998,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="635" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="635" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A635" t="s">
         <v>2114</v>
       </c>
@@ -46064,7 +46058,7 @@
         <v>11f2</v>
       </c>
     </row>
-    <row r="636" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="636" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A636" t="s">
         <v>2117</v>
       </c>
@@ -46124,7 +46118,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="637" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="637" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A637" t="s">
         <v>2120</v>
       </c>
@@ -46184,7 +46178,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="638" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="638" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A638" t="s">
         <v>2123</v>
       </c>
@@ -46244,7 +46238,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="639" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="639" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A639" t="s">
         <v>2126</v>
       </c>
@@ -46304,7 +46298,7 @@
         <v>11f3</v>
       </c>
     </row>
-    <row r="640" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="640" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A640" t="s">
         <v>2129</v>
       </c>
@@ -46364,7 +46358,7 @@
         <v>11f4</v>
       </c>
     </row>
-    <row r="641" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="641" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A641" t="s">
         <v>2132</v>
       </c>
@@ -46424,7 +46418,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="642" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="642" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A642" t="s">
         <v>2135</v>
       </c>
@@ -46484,7 +46478,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="643" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="643" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A643" t="s">
         <v>2138</v>
       </c>
@@ -46544,7 +46538,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="644" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="644" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A644" t="s">
         <v>2141</v>
       </c>
@@ -46604,7 +46598,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="645" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="645" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A645" t="s">
         <v>2144</v>
       </c>
@@ -46664,7 +46658,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="646" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="646" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A646" t="s">
         <v>2147</v>
       </c>
@@ -46724,7 +46718,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="647" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="647" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A647" t="s">
         <v>2150</v>
       </c>
@@ -46784,7 +46778,7 @@
         <v>11f5</v>
       </c>
     </row>
-    <row r="648" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
+    <row r="648" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A648" t="s">
         <v>2152</v>
       </c>

</xml_diff>

<commit_message>
Updates after the run
</commit_message>
<xml_diff>
--- a/JAF_indicators__definitions.xlsx
+++ b/JAF_indicators__definitions.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0" firstSheet="0" windowHeight="13125" windowWidth="13125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="compiled on 2024-03-07 11.25.37" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="compiled on 2024-03-08 09.20.56" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Comments" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
@@ -3050,7 +3050,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PA1.C20-29.M</t>
+          <t>PA1.C7.20-29.M</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3123,7 +3123,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PA1.C20-29.W</t>
+          <t>PA1.C7.20-29.W</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -23504,7 +23504,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>PA9.2.C4</t>
+          <t>PA9.2.C4.</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">

</xml_diff>

<commit_message>
Added lfse_er_child in EPM. Correction in definitions.
</commit_message>
<xml_diff>
--- a/JAF_indicators__definitions.xlsx
+++ b/JAF_indicators__definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/JAF2R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6C740E10149F00D2C464EA32ABA95ED2C55DD162" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0100709E-5FCC-443A-9564-102FF200A3F2}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_6C740E10149F00D2C464EA32ABA95ED2C55DD162" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECFAE5D8-C228-4AC2-B431-E67A638FDC07}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="21549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6965,30 +6965,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="jaf" displayName="jaf" ref="A2:K571" totalsRowShown="0">
   <autoFilter ref="A2:K571" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="10">
       <filters>
-        <filter val="fromFormula(a - b,_x000a_  where = variables(_x000a_  a = fromLFSspecialFile(&quot;lfse_er_child&quot;, _x000a_    with_filters(age = &quot;Y20-49&quot;, children = &quot;no&quot;, sex = &quot;F&quot;)),_x000a_  b = fromLFSspecialFile(&quot;lfse_er_child&quot;, _x000a_    with_filters(age = &quot;Y20-49&quot;, children = &quot;yes&quot;, sex = &quot;F&quot;))))"/>
-        <filter val="fromFormula(a - b,_x000a_  where = variables(_x000a_  a = fromLFSspecialFile(&quot;lfse_er_child&quot;, _x000a_    with_filters(age = &quot;Y20-49&quot;, children = &quot;no&quot;, sex = &quot;M&quot;)),_x000a_  b = fromLFSspecialFile(&quot;lfse_er_child&quot;, _x000a_    with_filters(age = &quot;Y20-49&quot;, children = &quot;yes&quot;, sex = &quot;M&quot;))))"/>
-        <filter val="fromFormula(a - b,_x000a_  where = variables(_x000a_  a = fromLFSspecialFile(&quot;lfse_er_child&quot;, _x000a_    with_filters(age = &quot;Y20-49&quot;, children = &quot;no&quot;, sex = &quot;T&quot;)),_x000a_  b = fromLFSspecialFile(&quot;lfse_er_child&quot;, _x000a_    with_filters(age = &quot;Y20-49&quot;, children = &quot;yes&quot;, sex = &quot;T&quot;))))"/>
-        <filter val="fromFormula(a - b,_x000a_  where = variables(_x000a_  a = fromLFSspecialFile(&quot;lfse_erfgap2064&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;M&quot;)),_x000a_  b = fromLFSspecialFile(&quot;lfse_erfgap2064&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;F&quot;))))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y15-64&quot;, sex = &quot;F&quot;, indicator = &quot;INACT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y15-64&quot;, sex = &quot;F&quot;, indicator = &quot;INACTPT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y15-64&quot;, sex = &quot;F&quot;, indicator = &quot;INACTPT_LACKCARE_ONFAMPERCARE&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y15-64&quot;, sex = &quot;F&quot;, indicator = &quot;PT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;F&quot;, indicator = &quot;INACTPT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;M&quot;, indicator = &quot;INACTPT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;T&quot;, indicator = &quot;INACT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;T&quot;, indicator = &quot;INACTPT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;T&quot;, indicator = &quot;INACTPT_LACKCARE_ONFAMPERCARE&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_inactpt_lackcare&quot;, _x000a_    with_filters(age = &quot;Y20-64&quot;, sex = &quot;T&quot;, indicator = &quot;PT_CARERESP_ONPOP&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_iscogap&quot;, _x000a_    with_filters(age = &quot;Y_GE15&quot;, sex = &quot;M&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_jobtenure&quot;, _x000a_    with_filters(age = &quot;Y15-64&quot;, sex = &quot;T&quot;, hatlev1d = &quot;TOTAL&quot;, indicator = &quot;hir_rate&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_jobtenure&quot;, _x000a_    with_filters(age = &quot;Y15-64&quot;, sex = &quot;T&quot;, hatlev1d = &quot;TOTAL&quot;, indicator = &quot;sep_rate&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_nacegap&quot;, _x000a_    with_filters(age = &quot;Y_GE15&quot;, sex = &quot;M&quot;))"/>
-        <filter val="fromLFSspecialFile(&quot;lfse_overtime&quot;, _x000a_    with_filters(sex = &quot;T&quot;, age = &quot;Y20-64&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_expenditure&quot;, _x000a_    with_filters(lmp_type = &quot;TOT11_7&quot;, exptype = &quot;XTOT&quot;, unit = &quot;PC_GDP&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_expenditure&quot;, _x000a_    with_filters(lmp_type = &quot;TOT11_7&quot;, exptype = &quot;XTOT&quot;, unit = &quot;PPS_PWW&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_ind_actime&quot;, _x000a_    with_filters(sex = &quot;T&quot;, unit = &quot;PC&quot;, lmp_type = &quot;TOT2_7&quot;, age = &quot;TOTAL&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_ind_actru&quot;, _x000a_    with_filters(sex = &quot;T&quot;, unit = &quot;RT&quot;, regis_es = &quot;REG_UNE&quot;, age = &quot;TOTAL&quot;, lmp_type = &quot;TOT2_7&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_ind_actru&quot;, _x000a_    with_filters(sex = &quot;T&quot;, unit = &quot;RT&quot;, regis_es = &quot;REG_UNE_LT&quot;, age = &quot;TOTAL&quot;, lmp_type = &quot;TOT2_7&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_ind_actsup&quot;, _x000a_    with_filters(sex = &quot;T&quot;, unit = &quot;RT&quot;, lmp_type = &quot;TOT2_7&quot;, age = &quot;TOTAL&quot;))"/>
+        <filter val="fromLMPdataset(&quot;lmp_ind_exp&quot;, _x000a_    with_filters(unit = &quot;PC_GDP&quot;, lmp_type = &quot;8&quot;))"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -7328,11 +7320,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S571"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A273" sqref="A165:A273"/>
+      <selection pane="bottomRight" activeCell="K177" sqref="K177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -17638,7 +17630,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
         <v>638</v>
       </c>
@@ -17701,7 +17693,7 @@
         <v>2b</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
         <v>642</v>
       </c>
@@ -18394,7 +18386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>681</v>
       </c>
@@ -18457,7 +18449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
         <v>686</v>
       </c>
@@ -18520,7 +18512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
         <v>690</v>
       </c>
@@ -18646,7 +18638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
         <v>699</v>
       </c>
@@ -18709,7 +18701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
         <v>703</v>
       </c>
@@ -18772,7 +18764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A183" t="s">
         <v>706</v>
       </c>
@@ -19465,7 +19457,7 @@
         <v>4.1</v>
       </c>
     </row>
-    <row r="194" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A194" t="s">
         <v>742</v>
       </c>
@@ -19906,7 +19898,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A201" t="s">
         <v>768</v>
       </c>
@@ -19969,7 +19961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A202" t="s">
         <v>772</v>
       </c>
@@ -20032,7 +20024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A203" t="s">
         <v>777</v>
       </c>
@@ -20095,7 +20087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A204" t="s">
         <v>780</v>
       </c>
@@ -20158,7 +20150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A205" t="s">
         <v>783</v>
       </c>
@@ -20221,7 +20213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A206" t="s">
         <v>786</v>
       </c>
@@ -20662,7 +20654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A213" t="s">
         <v>810</v>
       </c>
@@ -20725,7 +20717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A214" t="s">
         <v>813</v>
       </c>
@@ -20788,7 +20780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A215" t="s">
         <v>817</v>
       </c>
@@ -20851,7 +20843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A216" t="s">
         <v>820</v>
       </c>
@@ -20914,7 +20906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A217" t="s">
         <v>824</v>
       </c>
@@ -23371,7 +23363,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A256" t="s">
         <v>966</v>
       </c>
@@ -23560,7 +23552,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A259" t="s">
         <v>978</v>
       </c>
@@ -23812,7 +23804,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A263" t="s">
         <v>992</v>
       </c>
@@ -23938,7 +23930,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A265" t="s">
         <v>1001</v>
       </c>
@@ -24001,7 +23993,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A266" t="s">
         <v>1002</v>
       </c>
@@ -24379,7 +24371,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A272" t="s">
         <v>1017</v>
       </c>
@@ -24442,7 +24434,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:18" hidden="1" x14ac:dyDescent="0.4">
       <c r="A273" t="s">
         <v>1020</v>
       </c>

</xml_diff>